<commit_message>
Uploaded by Debasish on 27th Jun, 2018
</commit_message>
<xml_diff>
--- a/ApplicationTestData/AppData.xlsx
+++ b/ApplicationTestData/AppData.xlsx
@@ -4,34 +4,29 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226" filterPrivacy="1"/>
   <bookViews>
-    <workbookView activeTab="1" windowHeight="2355" windowWidth="14250" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="2" windowHeight="3840" windowWidth="14010" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
-    <sheet name="bldata" r:id="rId2" sheetId="2"/>
+    <sheet name="ContractData" r:id="rId2" sheetId="3"/>
+    <sheet name="bldata" r:id="rId3" sheetId="2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="48">
   <si>
     <t>ghoshd</t>
   </si>
   <si>
-    <t>molit@123</t>
-  </si>
-  <si>
     <t>Debasish</t>
   </si>
   <si>
     <t>Ghosh</t>
   </si>
   <si>
-    <t>18000004280</t>
-  </si>
-  <si>
     <t>Booking No:</t>
   </si>
   <si>
@@ -41,21 +36,140 @@
     <t>18000005899</t>
   </si>
   <si>
-    <t>TC1800418</t>
-  </si>
-  <si>
-    <t>TC1800419</t>
-  </si>
-  <si>
-    <t>TC1800420</t>
+    <t>molit@1234</t>
+  </si>
+  <si>
+    <t>Contract Type</t>
+  </si>
+  <si>
+    <t>Transport Contract</t>
+  </si>
+  <si>
+    <t>TransportContract_auto</t>
+  </si>
+  <si>
+    <t>Contract Effective Date</t>
+  </si>
+  <si>
+    <t>Contract Expiry Date</t>
+  </si>
+  <si>
+    <t>Contract Load Port</t>
+  </si>
+  <si>
+    <t>SGSINPP</t>
+  </si>
+  <si>
+    <t>Contract Dish port</t>
+  </si>
+  <si>
+    <t>HKHKGPC</t>
+  </si>
+  <si>
+    <t>Cargo Type</t>
+  </si>
+  <si>
+    <t>TRUCK</t>
+  </si>
+  <si>
+    <t>Make Name</t>
+  </si>
+  <si>
+    <t>Contract Name</t>
+  </si>
+  <si>
+    <t>Main Customer</t>
+  </si>
+  <si>
+    <t>ASHOK</t>
+  </si>
+  <si>
+    <t>Model Name</t>
+  </si>
+  <si>
+    <t>MINI TRUCK</t>
+  </si>
+  <si>
+    <t>Basis</t>
+  </si>
+  <si>
+    <t>PB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rate </t>
+  </si>
+  <si>
+    <t>Currency</t>
+  </si>
+  <si>
+    <t>SGD</t>
+  </si>
+  <si>
+    <t>Prepaid/Collect</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>Freight Collection Office</t>
+  </si>
+  <si>
+    <t>MOLSIN</t>
+  </si>
+  <si>
+    <t>Invoice Office</t>
+  </si>
+  <si>
+    <t>Payer</t>
+  </si>
+  <si>
+    <t>TC1800520</t>
+  </si>
+  <si>
+    <t>Booking Doc Entry Office</t>
+  </si>
+  <si>
+    <t>Booking Doc Issue Office</t>
+  </si>
+  <si>
+    <t>Consignee Number</t>
+  </si>
+  <si>
+    <t>Cargo Unit</t>
+  </si>
+  <si>
+    <t>B/L Data</t>
+  </si>
+  <si>
+    <t>Goods Description Text</t>
+  </si>
+  <si>
+    <t>Goods Description for Cargo Details One</t>
+  </si>
+  <si>
+    <t>TC1800530</t>
+  </si>
+  <si>
+    <t>TC1800531</t>
+  </si>
+  <si>
+    <t>TC1800532</t>
+  </si>
+  <si>
+    <t>TC1800534</t>
+  </si>
+  <si>
+    <t>TC1800537</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-409]dd\-mmm\-yy;@"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -67,6 +181,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -93,10 +215,18 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
@@ -405,7 +535,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -419,15 +549,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -440,44 +570,241 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C17"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="20.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="25.42578125" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3">
+        <v>5117553</v>
+      </c>
+    </row>
+    <row ht="30" r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="5">
+        <v>43214</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="5">
+        <v>43579</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row ht="30" r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17">
+        <v>5117553</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" customWidth="true" width="15.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="24.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="16.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="2">
+        <v>18000008178</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>7</v>
+      <c r="C3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3">
+        <v>5056735</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C4" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C9" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row ht="60" r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C10" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>